<commit_message>
Demo spreadsheet: Added format page
</commit_message>
<xml_diff>
--- a/import/DemoSpreadsheet.xlsx
+++ b/import/DemoSpreadsheet.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Documents\GitHub\MSTD\import_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/grantgiesbrecht/Documents/GitHub/Enceladus/import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB23ABDB-15AE-4551-BE48-857C3CE67B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B178A362-3592-A54A-A9FD-C35F1DC17A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1512" yWindow="1212" windowWidth="19668" windowHeight="10824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="10860" windowWidth="19660" windowHeight="10820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Day 2" sheetId="2" r:id="rId2"/>
+    <sheet name="S3" sheetId="3" r:id="rId3"/>
+    <sheet name="MATLABFormat" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>label 1</t>
   </si>
@@ -51,13 +53,76 @@
   </si>
   <si>
     <t>I mA</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Label 2</t>
+  </si>
+  <si>
+    <t>Label 3</t>
+  </si>
+  <si>
+    <t>Label 4</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>1. Find column before missing</t>
+  </si>
+  <si>
+    <t>2. ID row before missing</t>
+  </si>
+  <si>
+    <t>3. When extend column, check adjacent cells</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Demo1</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <t>Demo 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -71,6 +136,19 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,10 +171,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -319,9 +400,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -335,7 +416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -349,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>10</v>
       </c>
@@ -363,7 +444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>100</v>
       </c>
@@ -377,7 +458,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -391,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>1.5</v>
       </c>
@@ -405,7 +486,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>15</v>
       </c>
@@ -419,7 +500,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>150</v>
       </c>
@@ -445,18 +526,18 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -467,7 +548,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -478,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -489,7 +570,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -500,7 +581,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -509,6 +590,178 @@
       </c>
       <c r="C8" s="1">
         <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792AD1E7-D77D-4A45-A290-C3CCDACA2E63}">
+  <dimension ref="C2:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="27" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3">
+        <v>100</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E5" s="3">
+        <v>2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>12</v>
+      </c>
+      <c r="G5" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="3">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="13" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="3:11" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" s="3" customFormat="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AAAA88-FB8B-474C-AB15-2C85A1C3755C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>